<commit_message>
Improved handling of attributes, added README, added visualisation notebook
</commit_message>
<xml_diff>
--- a/data/decc/data_combination.xlsx
+++ b/data/decc/data_combination.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/decc-archive/data/decc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F53EDD1-D4EF-3743-A715-01BD760ACB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ED27C5-B7E1-ED4F-9F9D-0CF96CE65F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1100" windowWidth="27240" windowHeight="16440" xr2:uid="{9985A75E-EB26-5749-BA8E-B1A91FE63120}"/>
+    <workbookView xWindow="8820" yWindow="680" windowWidth="27240" windowHeight="16440" xr2:uid="{9985A75E-EB26-5749-BA8E-B1A91FE63120}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="13" r:id="rId1"/>
+    <sheet name="MHD" sheetId="14" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,10 +35,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Picarro end</t>
+  </si>
+  <si>
+    <t>Picarro start</t>
+  </si>
+  <si>
+    <t>GCMD end</t>
+  </si>
+  <si>
+    <t>GCMD start</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t># NOTE: ENSURE CELLS ARE FORMATTED AS TEXT, NOT DATES. IF PASTING VALUES ENSURE YOU "MATCH DESTINATION FORMATTING" TO PREVENT EXCEL FROM CONVERTING TO DATE AND TIME</t>
+  </si>
+  <si>
+    <t># Date format should be YYYY-MM-DD HH:MM</t>
+  </si>
+  <si>
+    <t># An "x" indicates that this instrument should not be included in timeseries for this species</t>
+  </si>
+  <si>
+    <t># Time periods can overlap if you want to keep both instruments</t>
+  </si>
+  <si>
+    <t># If there is no entry for a species it is assumed that it is only measured on the GCMS-Medusa</t>
+  </si>
+  <si>
+    <t># A blank entry in either the start or end date means that the time is unbounded at that side</t>
+  </si>
+  <si>
+    <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,8 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,15 +432,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4040417F-9A3B-E44E-944F-745B01BD7456}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767045A6-86CD-B442-8627-AB0BBFACEE63}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fill in spreadsheets and update scale_defaults.csv to align with agage-archive
</commit_message>
<xml_diff>
--- a/data/decc/data_combination.xlsx
+++ b/data/decc/data_combination.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/decc-archive/data/decc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp13716\user\home\zh21490\decc-archive\data\decc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ED27C5-B7E1-ED4F-9F9D-0CF96CE65F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6EFB0E-5D76-4CFF-8686-0ECBAF20B918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="680" windowWidth="27240" windowHeight="16440" xr2:uid="{9985A75E-EB26-5749-BA8E-B1A91FE63120}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9985A75E-EB26-5749-BA8E-B1A91FE63120}"/>
   </bookViews>
   <sheets>
-    <sheet name="MHD" sheetId="14" r:id="rId1"/>
+    <sheet name="BSD" sheetId="14" r:id="rId1"/>
+    <sheet name="HFD" sheetId="15" r:id="rId2"/>
+    <sheet name="JBO" sheetId="16" r:id="rId3"/>
+    <sheet name="RGL" sheetId="17" r:id="rId4"/>
+    <sheet name="SIS" sheetId="18" r:id="rId5"/>
+    <sheet name="TTA" sheetId="19" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,13 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Picarro end</t>
-  </si>
-  <si>
-    <t>Picarro start</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
   <si>
     <t>GCMD end</t>
   </si>
@@ -72,6 +71,42 @@
   </si>
   <si>
     <t># File specifying when to use the various ALE/GAGE/AGAGE instruments</t>
+  </si>
+  <si>
+    <t>Picarro-G5310 start</t>
+  </si>
+  <si>
+    <t>Picarro-G5310 end</t>
+  </si>
+  <si>
+    <t>n2o</t>
+  </si>
+  <si>
+    <t>co</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>2019-03-06 12:00</t>
+  </si>
+  <si>
+    <t>Picarro-G2401 start</t>
+  </si>
+  <si>
+    <t>Picarro-G2401 end</t>
+  </si>
+  <si>
+    <t>Picarro-G2301 start</t>
+  </si>
+  <si>
+    <t>Picarro-G2301 end</t>
+  </si>
+  <si>
+    <t>2019-03-06 11:59</t>
+  </si>
+  <si>
+    <t>2023-10-19 16:59</t>
   </si>
 </sst>
 </file>
@@ -433,70 +468,498 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767045A6-86CD-B442-8627-AB0BBFACEE63}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="3" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E25449-DA0F-49AE-837A-375C3D7581EE}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1"/>
+    <col min="2" max="3" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069C7DF1-C0F3-455C-95BB-588F8E029510}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1"/>
+    <col min="2" max="2" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB5102E-72EF-4DAE-B68F-D2D57BC6339A}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1"/>
+    <col min="2" max="3" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD390D53-465D-4CA9-BAF6-778BB482F172}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F14:F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1"/>
+    <col min="2" max="2" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF3ACA6-7478-4B73-869D-7B31806D141B}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="11" style="1"/>
+    <col min="2" max="2" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>